<commit_message>
Actualización del plan general.
</commit_message>
<xml_diff>
--- a/tspi/ciclo-1/logt1/20095495.xlsx
+++ b/tspi/ciclo-1/logt1/20095495.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -62,7 +62,10 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Realizar el lanzamiento del ciclo #1 de TSPi.</t>
+  </si>
+  <si>
+    <t>Definir la estrategía de desarrollo del ciclo #1 de TSPi.</t>
   </si>
   <si>
     <t>Video tutorial de Github.</t>
@@ -222,7 +225,7 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -241,21 +244,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E9" activeCellId="0" pane="topLeft" sqref="E9"/>
+      <selection activeCell="E6" activeCellId="0" pane="topLeft" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="11.8313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="16.5882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.8156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.3960784313726"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="11.8313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="46.7490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="11.8313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="11.8941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="16.6705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.8705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="11.8941176470588"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="46.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="4" width="11.8941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="1">
@@ -270,7 +273,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="9" t="n">
-        <v>41898</v>
+        <v>41902</v>
       </c>
       <c r="G1" s="9"/>
     </row>
@@ -304,78 +307,109 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5">
-      <c r="A5" s="12" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
+      <c r="E5" s="3" t="n">
+        <f aca="false">SUM(E7:E9)/60</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
+      <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
-      <c r="A6" s="1" t="n">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="7">
+      <c r="A7" s="1" t="n">
+        <v>41902</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.631944444444444</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.684027777777778</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <f aca="false">((HOUR(C7)-HOUR(B7))*60)+(MINUTE(C7)-MINUTE(B7))-D7</f>
+        <v>61</v>
+      </c>
+      <c r="F7" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="8">
+      <c r="A8" s="1" t="n">
+        <v>41902</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0.725694444444444</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <f aca="false">((HOUR(C8)-HOUR(B8))*60)+(MINUTE(C8)-MINUTE(B8))-D8</f>
+        <v>45</v>
+      </c>
+      <c r="F8" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="9">
+      <c r="A9" s="1" t="n">
         <v>41904</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B9" s="2" t="n">
         <v>0.340277777777778</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C9" s="2" t="n">
         <v>0.354166666666667</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D9" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="n">
-        <f aca="false">((HOUR(C6)-HOUR(B6))*60)+(MINUTE(C6)-MINUTE(B6))-D6</f>
+      <c r="E9" s="3" t="n">
+        <f aca="false">((HOUR(C9)-HOUR(B9))*60)+(MINUTE(C9)-MINUTE(B9))-D9</f>
         <v>20</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="7">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="8">
-      <c r="A8" s="0"/>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0" t="n">
-        <f aca="false">SUM(E6:E7)/60</f>
-        <v>0.333333333333333</v>
-      </c>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
+      <c r="F9" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>